<commit_message>
Actualizo datos en PuertoMontt.xlsx
</commit_message>
<xml_diff>
--- a/PuertoMontt.xlsx
+++ b/PuertoMontt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathan.diaz/Desktop/Programación/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60F66E42-566D-D549-8152-0D3E86B17BB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{741A9E55-84E2-F942-AEBE-4A9F8B756977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -476,7 +476,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2271" uniqueCount="938">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2311" uniqueCount="958">
   <si>
     <t>Temperature(℃)</t>
   </si>
@@ -3291,6 +3291,66 @@
   <si>
     <t>2025-03-31 17:00</t>
   </si>
+  <si>
+    <t>2025-08-01 00:00</t>
+  </si>
+  <si>
+    <t>2025-08-01 04:00</t>
+  </si>
+  <si>
+    <t>2025-08-01 08:00</t>
+  </si>
+  <si>
+    <t>2025-08-01 12:00</t>
+  </si>
+  <si>
+    <t>2025-08-01 16:00</t>
+  </si>
+  <si>
+    <t>2025-08-01 20:00</t>
+  </si>
+  <si>
+    <t>2025-08-02 00:00</t>
+  </si>
+  <si>
+    <t>2025-08-02 04:00</t>
+  </si>
+  <si>
+    <t>2025-08-02 08:00</t>
+  </si>
+  <si>
+    <t>2025-08-02 12:00</t>
+  </si>
+  <si>
+    <t>2025-08-02 16:00</t>
+  </si>
+  <si>
+    <t>2025-08-02 20:00</t>
+  </si>
+  <si>
+    <t>2025-08-03 00:00</t>
+  </si>
+  <si>
+    <t>2025-08-03 04:00</t>
+  </si>
+  <si>
+    <t>2025-08-03 08:00</t>
+  </si>
+  <si>
+    <t>2025-08-03 12:00</t>
+  </si>
+  <si>
+    <t>2025-08-03 16:00</t>
+  </si>
+  <si>
+    <t>2025-08-03 20:00</t>
+  </si>
+  <si>
+    <t>2025-08-04 00:00</t>
+  </si>
+  <si>
+    <t>2025-08-04 04:00</t>
+  </si>
 </sst>
 </file>
 
@@ -3894,13 +3954,13 @@
   <sheetPr>
     <tabColor rgb="FF0094FF"/>
   </sheetPr>
-  <dimension ref="A1:AI909"/>
+  <dimension ref="A1:AI929"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B241" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B889" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A910" sqref="A910:XFD929"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -96806,7 +96866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="897" spans="1:33" ht="18" customHeight="1">
+    <row r="897" spans="1:35" ht="18" customHeight="1">
       <c r="A897" s="11" t="s">
         <v>92</v>
       </c>
@@ -96907,7 +96967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="898" spans="1:33" ht="18" customHeight="1">
+    <row r="898" spans="1:35" ht="18" customHeight="1">
       <c r="A898" s="2" t="s">
         <v>928</v>
       </c>
@@ -97008,7 +97068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="899" spans="1:33" ht="18" customHeight="1">
+    <row r="899" spans="1:35" ht="18" customHeight="1">
       <c r="A899" s="11" t="s">
         <v>929</v>
       </c>
@@ -97109,7 +97169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="900" spans="1:33" ht="18" customHeight="1">
+    <row r="900" spans="1:35" ht="18" customHeight="1">
       <c r="A900" s="2" t="s">
         <v>930</v>
       </c>
@@ -97210,7 +97270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="901" spans="1:33" ht="18" customHeight="1">
+    <row r="901" spans="1:35" ht="18" customHeight="1">
       <c r="A901" s="11" t="s">
         <v>931</v>
       </c>
@@ -97311,7 +97371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="902" spans="1:33" ht="18" customHeight="1">
+    <row r="902" spans="1:35" ht="18" customHeight="1">
       <c r="A902" s="2" t="s">
         <v>932</v>
       </c>
@@ -97412,7 +97472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="903" spans="1:33" ht="18" customHeight="1">
+    <row r="903" spans="1:35" ht="18" customHeight="1">
       <c r="A903" s="11" t="s">
         <v>93</v>
       </c>
@@ -97513,7 +97573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="904" spans="1:33" ht="18" customHeight="1">
+    <row r="904" spans="1:35" ht="18" customHeight="1">
       <c r="A904" s="2" t="s">
         <v>933</v>
       </c>
@@ -97614,7 +97674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="905" spans="1:33" ht="18" customHeight="1">
+    <row r="905" spans="1:35" ht="18" customHeight="1">
       <c r="A905" s="11" t="s">
         <v>934</v>
       </c>
@@ -97715,7 +97775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="906" spans="1:33" ht="18" customHeight="1">
+    <row r="906" spans="1:35" ht="18" customHeight="1">
       <c r="A906" s="2" t="s">
         <v>935</v>
       </c>
@@ -97816,7 +97876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="907" spans="1:33" ht="18" customHeight="1">
+    <row r="907" spans="1:35" ht="18" customHeight="1">
       <c r="A907" s="11" t="s">
         <v>936</v>
       </c>
@@ -97917,7 +97977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="908" spans="1:33" ht="18" customHeight="1">
+    <row r="908" spans="1:35" ht="18" customHeight="1">
       <c r="A908" s="2" t="s">
         <v>937</v>
       </c>
@@ -98018,7 +98078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="909" spans="1:33" ht="18" customHeight="1">
+    <row r="909" spans="1:35" ht="18" customHeight="1">
       <c r="A909" s="16" t="s">
         <v>94</v>
       </c>
@@ -98116,6 +98176,2146 @@
         <v>1012.4</v>
       </c>
       <c r="AG909" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="910" spans="1:35" ht="18" customHeight="1">
+      <c r="A910" s="1" t="s">
+        <v>938</v>
+      </c>
+      <c r="B910" s="3">
+        <v>13</v>
+      </c>
+      <c r="C910" s="3">
+        <v>12.4</v>
+      </c>
+      <c r="D910" s="3">
+        <v>13.8</v>
+      </c>
+      <c r="E910" s="3">
+        <v>13</v>
+      </c>
+      <c r="F910" s="3">
+        <v>12.9</v>
+      </c>
+      <c r="G910" s="4">
+        <v>99</v>
+      </c>
+      <c r="H910" s="4">
+        <v>99</v>
+      </c>
+      <c r="I910" s="4">
+        <v>99</v>
+      </c>
+      <c r="J910" s="3">
+        <v>15.9</v>
+      </c>
+      <c r="K910" s="3">
+        <v>15.3</v>
+      </c>
+      <c r="L910" s="3">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="M910" s="4">
+        <v>70</v>
+      </c>
+      <c r="N910" s="4">
+        <v>68</v>
+      </c>
+      <c r="O910" s="4">
+        <v>71</v>
+      </c>
+      <c r="P910" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q910" s="4">
+        <v>0</v>
+      </c>
+      <c r="R910" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="S910" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="T910" s="3">
+        <v>185.4</v>
+      </c>
+      <c r="U910" s="3">
+        <v>0</v>
+      </c>
+      <c r="V910" s="3">
+        <v>184.4</v>
+      </c>
+      <c r="W910" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="X910" s="3">
+        <v>1213.7</v>
+      </c>
+      <c r="Y910" s="3">
+        <v>22.2</v>
+      </c>
+      <c r="Z910" s="3">
+        <v>51.5</v>
+      </c>
+      <c r="AA910" s="4">
+        <v>11</v>
+      </c>
+      <c r="AB910" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC910" s="3">
+        <v>991.5</v>
+      </c>
+      <c r="AD910" s="3">
+        <v>990.6</v>
+      </c>
+      <c r="AE910" s="3">
+        <v>992.5</v>
+      </c>
+      <c r="AF910" s="3">
+        <v>991.5</v>
+      </c>
+      <c r="AG910" s="4">
+        <v>72260</v>
+      </c>
+      <c r="AH910" s="4">
+        <v>7430449</v>
+      </c>
+      <c r="AI910" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="911" spans="1:35" ht="18" customHeight="1">
+      <c r="A911" s="11" t="s">
+        <v>939</v>
+      </c>
+      <c r="B911" s="12">
+        <v>13.4</v>
+      </c>
+      <c r="C911" s="12">
+        <v>12.4</v>
+      </c>
+      <c r="D911" s="12">
+        <v>14.1</v>
+      </c>
+      <c r="E911" s="12">
+        <v>13.4</v>
+      </c>
+      <c r="F911" s="12">
+        <v>13.2</v>
+      </c>
+      <c r="G911" s="13">
+        <v>99</v>
+      </c>
+      <c r="H911" s="13">
+        <v>99</v>
+      </c>
+      <c r="I911" s="13">
+        <v>99</v>
+      </c>
+      <c r="J911" s="12">
+        <v>15.2</v>
+      </c>
+      <c r="K911" s="12">
+        <v>15.1</v>
+      </c>
+      <c r="L911" s="12">
+        <v>15.4</v>
+      </c>
+      <c r="M911" s="13">
+        <v>67</v>
+      </c>
+      <c r="N911" s="13">
+        <v>64</v>
+      </c>
+      <c r="O911" s="13">
+        <v>70</v>
+      </c>
+      <c r="P911" s="12">
+        <v>1.6</v>
+      </c>
+      <c r="Q911" s="13">
+        <v>0</v>
+      </c>
+      <c r="R911" s="12">
+        <v>0</v>
+      </c>
+      <c r="S911" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="T911" s="12">
+        <v>185.4</v>
+      </c>
+      <c r="U911" s="12">
+        <v>0</v>
+      </c>
+      <c r="V911" s="12">
+        <v>184.4</v>
+      </c>
+      <c r="W911" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="X911" s="12">
+        <v>1213.7</v>
+      </c>
+      <c r="Y911" s="12">
+        <v>30.5</v>
+      </c>
+      <c r="Z911" s="12">
+        <v>84.6</v>
+      </c>
+      <c r="AA911" s="13">
+        <v>14</v>
+      </c>
+      <c r="AB911" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC911" s="12">
+        <v>990.1</v>
+      </c>
+      <c r="AD911" s="12">
+        <v>989.4</v>
+      </c>
+      <c r="AE911" s="12">
+        <v>991</v>
+      </c>
+      <c r="AF911" s="12">
+        <v>990.1</v>
+      </c>
+      <c r="AG911" s="13">
+        <v>72596</v>
+      </c>
+      <c r="AH911" s="13">
+        <v>7444848</v>
+      </c>
+      <c r="AI911" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="912" spans="1:35" ht="18" customHeight="1">
+      <c r="A912" s="2" t="s">
+        <v>940</v>
+      </c>
+      <c r="B912" s="6">
+        <v>12</v>
+      </c>
+      <c r="C912" s="6">
+        <v>10.5</v>
+      </c>
+      <c r="D912" s="6">
+        <v>13.6</v>
+      </c>
+      <c r="E912" s="6">
+        <v>12</v>
+      </c>
+      <c r="F912" s="6">
+        <v>11.8</v>
+      </c>
+      <c r="G912" s="7">
+        <v>99</v>
+      </c>
+      <c r="H912" s="7">
+        <v>99</v>
+      </c>
+      <c r="I912" s="7">
+        <v>99</v>
+      </c>
+      <c r="J912" s="6">
+        <v>16.5</v>
+      </c>
+      <c r="K912" s="6">
+        <v>15.3</v>
+      </c>
+      <c r="L912" s="6">
+        <v>17.8</v>
+      </c>
+      <c r="M912" s="7">
+        <v>66</v>
+      </c>
+      <c r="N912" s="7">
+        <v>64</v>
+      </c>
+      <c r="O912" s="7">
+        <v>68</v>
+      </c>
+      <c r="P912" s="6">
+        <v>205.3</v>
+      </c>
+      <c r="Q912" s="7">
+        <v>2</v>
+      </c>
+      <c r="R912" s="6">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="S912" s="6">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="T912" s="6">
+        <v>187.4</v>
+      </c>
+      <c r="U912" s="6">
+        <v>0</v>
+      </c>
+      <c r="V912" s="6">
+        <v>186.4</v>
+      </c>
+      <c r="W912" s="6">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="X912" s="6">
+        <v>1215.7</v>
+      </c>
+      <c r="Y912" s="6">
+        <v>28.4</v>
+      </c>
+      <c r="Z912" s="6">
+        <v>78.8</v>
+      </c>
+      <c r="AA912" s="7">
+        <v>7</v>
+      </c>
+      <c r="AB912" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC912" s="6">
+        <v>993.5</v>
+      </c>
+      <c r="AD912" s="6">
+        <v>990.8</v>
+      </c>
+      <c r="AE912" s="6">
+        <v>996.4</v>
+      </c>
+      <c r="AF912" s="6">
+        <v>993.5</v>
+      </c>
+      <c r="AG912" s="7">
+        <v>72596</v>
+      </c>
+      <c r="AH912" s="7">
+        <v>7459241</v>
+      </c>
+      <c r="AI912" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="913" spans="1:35" ht="18" customHeight="1">
+      <c r="A913" s="11" t="s">
+        <v>941</v>
+      </c>
+      <c r="B913" s="12">
+        <v>12.6</v>
+      </c>
+      <c r="C913" s="12">
+        <v>11.7</v>
+      </c>
+      <c r="D913" s="12">
+        <v>13.1</v>
+      </c>
+      <c r="E913" s="12">
+        <v>12.6</v>
+      </c>
+      <c r="F913" s="12">
+        <v>12.5</v>
+      </c>
+      <c r="G913" s="13">
+        <v>99</v>
+      </c>
+      <c r="H913" s="13">
+        <v>99</v>
+      </c>
+      <c r="I913" s="13">
+        <v>99</v>
+      </c>
+      <c r="J913" s="12">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="K913" s="12">
+        <v>17.8</v>
+      </c>
+      <c r="L913" s="12">
+        <v>19.5</v>
+      </c>
+      <c r="M913" s="13">
+        <v>64</v>
+      </c>
+      <c r="N913" s="13">
+        <v>62</v>
+      </c>
+      <c r="O913" s="13">
+        <v>66</v>
+      </c>
+      <c r="P913" s="12">
+        <v>561.4</v>
+      </c>
+      <c r="Q913" s="13">
+        <v>5</v>
+      </c>
+      <c r="R913" s="12">
+        <v>0</v>
+      </c>
+      <c r="S913" s="12">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="T913" s="12">
+        <v>187.4</v>
+      </c>
+      <c r="U913" s="12">
+        <v>0</v>
+      </c>
+      <c r="V913" s="12">
+        <v>186.4</v>
+      </c>
+      <c r="W913" s="12">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="X913" s="12">
+        <v>1215.7</v>
+      </c>
+      <c r="Y913" s="12">
+        <v>14.5</v>
+      </c>
+      <c r="Z913" s="12">
+        <v>40.299999999999997</v>
+      </c>
+      <c r="AA913" s="13">
+        <v>3</v>
+      </c>
+      <c r="AB913" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC913" s="12">
+        <v>995.6</v>
+      </c>
+      <c r="AD913" s="12">
+        <v>994.9</v>
+      </c>
+      <c r="AE913" s="12">
+        <v>996.2</v>
+      </c>
+      <c r="AF913" s="12">
+        <v>995.6</v>
+      </c>
+      <c r="AG913" s="13">
+        <v>72592</v>
+      </c>
+      <c r="AH913" s="13">
+        <v>7473637</v>
+      </c>
+      <c r="AI913" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="914" spans="1:35" ht="18" customHeight="1">
+      <c r="A914" s="2" t="s">
+        <v>942</v>
+      </c>
+      <c r="B914" s="6">
+        <v>9.6</v>
+      </c>
+      <c r="C914" s="6">
+        <v>8.5</v>
+      </c>
+      <c r="D914" s="6">
+        <v>12.4</v>
+      </c>
+      <c r="E914" s="6">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="F914" s="6">
+        <v>9.5</v>
+      </c>
+      <c r="G914" s="7">
+        <v>99</v>
+      </c>
+      <c r="H914" s="7">
+        <v>99</v>
+      </c>
+      <c r="I914" s="7">
+        <v>99</v>
+      </c>
+      <c r="J914" s="6">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="K914" s="6">
+        <v>17.5</v>
+      </c>
+      <c r="L914" s="6">
+        <v>19.5</v>
+      </c>
+      <c r="M914" s="7">
+        <v>67</v>
+      </c>
+      <c r="N914" s="7">
+        <v>64</v>
+      </c>
+      <c r="O914" s="7">
+        <v>68</v>
+      </c>
+      <c r="P914" s="6">
+        <v>64.3</v>
+      </c>
+      <c r="Q914" s="7">
+        <v>0</v>
+      </c>
+      <c r="R914" s="6">
+        <v>48.6</v>
+      </c>
+      <c r="S914" s="6">
+        <v>61.2</v>
+      </c>
+      <c r="T914" s="6">
+        <v>246.4</v>
+      </c>
+      <c r="U914" s="6">
+        <v>9.4</v>
+      </c>
+      <c r="V914" s="6">
+        <v>245.4</v>
+      </c>
+      <c r="W914" s="6">
+        <v>61.2</v>
+      </c>
+      <c r="X914" s="6">
+        <v>1274.7</v>
+      </c>
+      <c r="Y914" s="6">
+        <v>5.9</v>
+      </c>
+      <c r="Z914" s="6">
+        <v>22</v>
+      </c>
+      <c r="AA914" s="7">
+        <v>70</v>
+      </c>
+      <c r="AB914" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC914" s="6">
+        <v>996.7</v>
+      </c>
+      <c r="AD914" s="6">
+        <v>995.5</v>
+      </c>
+      <c r="AE914" s="6">
+        <v>997.9</v>
+      </c>
+      <c r="AF914" s="6">
+        <v>996.7</v>
+      </c>
+      <c r="AG914" s="7">
+        <v>106620</v>
+      </c>
+      <c r="AH914" s="7">
+        <v>7488033</v>
+      </c>
+      <c r="AI914" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="915" spans="1:35" ht="18" customHeight="1">
+      <c r="A915" s="11" t="s">
+        <v>943</v>
+      </c>
+      <c r="B915" s="12">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="C915" s="12">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="D915" s="12">
+        <v>9.1</v>
+      </c>
+      <c r="E915" s="12">
+        <v>7</v>
+      </c>
+      <c r="F915" s="12">
+        <v>8.5</v>
+      </c>
+      <c r="G915" s="13">
+        <v>99</v>
+      </c>
+      <c r="H915" s="13">
+        <v>99</v>
+      </c>
+      <c r="I915" s="13">
+        <v>99</v>
+      </c>
+      <c r="J915" s="12">
+        <v>16.8</v>
+      </c>
+      <c r="K915" s="12">
+        <v>16</v>
+      </c>
+      <c r="L915" s="12">
+        <v>17.5</v>
+      </c>
+      <c r="M915" s="13">
+        <v>68</v>
+      </c>
+      <c r="N915" s="13">
+        <v>66</v>
+      </c>
+      <c r="O915" s="13">
+        <v>71</v>
+      </c>
+      <c r="P915" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q915" s="13">
+        <v>0</v>
+      </c>
+      <c r="R915" s="12">
+        <v>13.8</v>
+      </c>
+      <c r="S915" s="12">
+        <v>72.599999999999994</v>
+      </c>
+      <c r="T915" s="12">
+        <v>257.8</v>
+      </c>
+      <c r="U915" s="12">
+        <v>2.8</v>
+      </c>
+      <c r="V915" s="12">
+        <v>256.8</v>
+      </c>
+      <c r="W915" s="12">
+        <v>72.599999999999994</v>
+      </c>
+      <c r="X915" s="12">
+        <v>1286.0999999999999</v>
+      </c>
+      <c r="Y915" s="12">
+        <v>10.8</v>
+      </c>
+      <c r="Z915" s="12">
+        <v>27.7</v>
+      </c>
+      <c r="AA915" s="13">
+        <v>28</v>
+      </c>
+      <c r="AB915" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC915" s="12">
+        <v>997.9</v>
+      </c>
+      <c r="AD915" s="12">
+        <v>997.3</v>
+      </c>
+      <c r="AE915" s="12">
+        <v>998.5</v>
+      </c>
+      <c r="AF915" s="12">
+        <v>997.9</v>
+      </c>
+      <c r="AG915" s="13">
+        <v>106648</v>
+      </c>
+      <c r="AH915" s="13">
+        <v>7502429</v>
+      </c>
+      <c r="AI915" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="916" spans="1:35" ht="18" customHeight="1">
+      <c r="A916" s="2" t="s">
+        <v>944</v>
+      </c>
+      <c r="B916" s="6">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="C916" s="6">
+        <v>7.2</v>
+      </c>
+      <c r="D916" s="6">
+        <v>9.1</v>
+      </c>
+      <c r="E916" s="6">
+        <v>6</v>
+      </c>
+      <c r="F916" s="6">
+        <v>8.1</v>
+      </c>
+      <c r="G916" s="7">
+        <v>99</v>
+      </c>
+      <c r="H916" s="7">
+        <v>99</v>
+      </c>
+      <c r="I916" s="7">
+        <v>99</v>
+      </c>
+      <c r="J916" s="6">
+        <v>15.4</v>
+      </c>
+      <c r="K916" s="6">
+        <v>14.9</v>
+      </c>
+      <c r="L916" s="6">
+        <v>16</v>
+      </c>
+      <c r="M916" s="7">
+        <v>72</v>
+      </c>
+      <c r="N916" s="7">
+        <v>71</v>
+      </c>
+      <c r="O916" s="7">
+        <v>72</v>
+      </c>
+      <c r="P916" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q916" s="7">
+        <v>0</v>
+      </c>
+      <c r="R916" s="6">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="S916" s="6">
+        <v>11.2</v>
+      </c>
+      <c r="T916" s="6">
+        <v>269</v>
+      </c>
+      <c r="U916" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="V916" s="6">
+        <v>268</v>
+      </c>
+      <c r="W916" s="6">
+        <v>83.8</v>
+      </c>
+      <c r="X916" s="6">
+        <v>1297.3</v>
+      </c>
+      <c r="Y916" s="6">
+        <v>13.5</v>
+      </c>
+      <c r="Z916" s="6">
+        <v>33.1</v>
+      </c>
+      <c r="AA916" s="7">
+        <v>256</v>
+      </c>
+      <c r="AB916" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC916" s="6">
+        <v>999</v>
+      </c>
+      <c r="AD916" s="6">
+        <v>998</v>
+      </c>
+      <c r="AE916" s="6">
+        <v>1000.2</v>
+      </c>
+      <c r="AF916" s="6">
+        <v>999</v>
+      </c>
+      <c r="AG916" s="7">
+        <v>106460</v>
+      </c>
+      <c r="AH916" s="7">
+        <v>7516825</v>
+      </c>
+      <c r="AI916" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="917" spans="1:35" ht="18" customHeight="1">
+      <c r="A917" s="11" t="s">
+        <v>945</v>
+      </c>
+      <c r="B917" s="12">
+        <v>6.8</v>
+      </c>
+      <c r="C917" s="12">
+        <v>5.6</v>
+      </c>
+      <c r="D917" s="12">
+        <v>7.3</v>
+      </c>
+      <c r="E917" s="12">
+        <v>5</v>
+      </c>
+      <c r="F917" s="12">
+        <v>6.7</v>
+      </c>
+      <c r="G917" s="13">
+        <v>99</v>
+      </c>
+      <c r="H917" s="13">
+        <v>99</v>
+      </c>
+      <c r="I917" s="13">
+        <v>99</v>
+      </c>
+      <c r="J917" s="12">
+        <v>14.4</v>
+      </c>
+      <c r="K917" s="12">
+        <v>13.7</v>
+      </c>
+      <c r="L917" s="12">
+        <v>14.9</v>
+      </c>
+      <c r="M917" s="13">
+        <v>71</v>
+      </c>
+      <c r="N917" s="13">
+        <v>70</v>
+      </c>
+      <c r="O917" s="13">
+        <v>72</v>
+      </c>
+      <c r="P917" s="12">
+        <v>3.8</v>
+      </c>
+      <c r="Q917" s="13">
+        <v>0</v>
+      </c>
+      <c r="R917" s="12">
+        <v>3</v>
+      </c>
+      <c r="S917" s="12">
+        <v>11.7</v>
+      </c>
+      <c r="T917" s="12">
+        <v>269.5</v>
+      </c>
+      <c r="U917" s="12">
+        <v>0</v>
+      </c>
+      <c r="V917" s="12">
+        <v>268.5</v>
+      </c>
+      <c r="W917" s="12">
+        <v>84.3</v>
+      </c>
+      <c r="X917" s="12">
+        <v>1297.8</v>
+      </c>
+      <c r="Y917" s="12">
+        <v>10.3</v>
+      </c>
+      <c r="Z917" s="12">
+        <v>29.5</v>
+      </c>
+      <c r="AA917" s="13">
+        <v>242</v>
+      </c>
+      <c r="AB917" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC917" s="12">
+        <v>1001.7</v>
+      </c>
+      <c r="AD917" s="12">
+        <v>999.9</v>
+      </c>
+      <c r="AE917" s="12">
+        <v>1003.7</v>
+      </c>
+      <c r="AF917" s="12">
+        <v>1001.7</v>
+      </c>
+      <c r="AG917" s="13">
+        <v>106436</v>
+      </c>
+      <c r="AH917" s="13">
+        <v>7531221</v>
+      </c>
+      <c r="AI917" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="918" spans="1:35" ht="18" customHeight="1">
+      <c r="A918" s="2" t="s">
+        <v>946</v>
+      </c>
+      <c r="B918" s="6">
+        <v>5.2</v>
+      </c>
+      <c r="C918" s="6">
+        <v>4.2</v>
+      </c>
+      <c r="D918" s="6">
+        <v>6.7</v>
+      </c>
+      <c r="E918" s="6">
+        <v>3.3</v>
+      </c>
+      <c r="F918" s="6">
+        <v>5</v>
+      </c>
+      <c r="G918" s="7">
+        <v>99</v>
+      </c>
+      <c r="H918" s="7">
+        <v>99</v>
+      </c>
+      <c r="I918" s="7">
+        <v>99</v>
+      </c>
+      <c r="J918" s="6">
+        <v>15.3</v>
+      </c>
+      <c r="K918" s="6">
+        <v>13.7</v>
+      </c>
+      <c r="L918" s="6">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="M918" s="7">
+        <v>72</v>
+      </c>
+      <c r="N918" s="7">
+        <v>69</v>
+      </c>
+      <c r="O918" s="7">
+        <v>79</v>
+      </c>
+      <c r="P918" s="6">
+        <v>468.4</v>
+      </c>
+      <c r="Q918" s="7">
+        <v>4</v>
+      </c>
+      <c r="R918" s="6">
+        <v>3</v>
+      </c>
+      <c r="S918" s="6">
+        <v>13.2</v>
+      </c>
+      <c r="T918" s="6">
+        <v>271</v>
+      </c>
+      <c r="U918" s="6">
+        <v>0</v>
+      </c>
+      <c r="V918" s="6">
+        <v>270</v>
+      </c>
+      <c r="W918" s="6">
+        <v>85.8</v>
+      </c>
+      <c r="X918" s="6">
+        <v>1299.3</v>
+      </c>
+      <c r="Y918" s="6">
+        <v>9.4</v>
+      </c>
+      <c r="Z918" s="6">
+        <v>34.9</v>
+      </c>
+      <c r="AA918" s="7">
+        <v>289</v>
+      </c>
+      <c r="AB918" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC918" s="6">
+        <v>1005</v>
+      </c>
+      <c r="AD918" s="6">
+        <v>1003.6</v>
+      </c>
+      <c r="AE918" s="6">
+        <v>1005.9</v>
+      </c>
+      <c r="AF918" s="6">
+        <v>1005</v>
+      </c>
+      <c r="AG918" s="7">
+        <v>106632</v>
+      </c>
+      <c r="AH918" s="7">
+        <v>7545618</v>
+      </c>
+      <c r="AI918" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="919" spans="1:35" ht="18" customHeight="1">
+      <c r="A919" s="11" t="s">
+        <v>947</v>
+      </c>
+      <c r="B919" s="12">
+        <v>7.1</v>
+      </c>
+      <c r="C919" s="12">
+        <v>5.2</v>
+      </c>
+      <c r="D919" s="12">
+        <v>9.6</v>
+      </c>
+      <c r="E919" s="12">
+        <v>5.8</v>
+      </c>
+      <c r="F919" s="12">
+        <v>7</v>
+      </c>
+      <c r="G919" s="13">
+        <v>99</v>
+      </c>
+      <c r="H919" s="13">
+        <v>99</v>
+      </c>
+      <c r="I919" s="13">
+        <v>99</v>
+      </c>
+      <c r="J919" s="12">
+        <v>18</v>
+      </c>
+      <c r="K919" s="12">
+        <v>17.7</v>
+      </c>
+      <c r="L919" s="12">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="M919" s="13">
+        <v>65</v>
+      </c>
+      <c r="N919" s="13">
+        <v>62</v>
+      </c>
+      <c r="O919" s="13">
+        <v>74</v>
+      </c>
+      <c r="P919" s="12">
+        <v>664.3</v>
+      </c>
+      <c r="Q919" s="13">
+        <v>6</v>
+      </c>
+      <c r="R919" s="12">
+        <v>1.8</v>
+      </c>
+      <c r="S919" s="12">
+        <v>13.7</v>
+      </c>
+      <c r="T919" s="12">
+        <v>271.5</v>
+      </c>
+      <c r="U919" s="12">
+        <v>0</v>
+      </c>
+      <c r="V919" s="12">
+        <v>270.5</v>
+      </c>
+      <c r="W919" s="12">
+        <v>86.3</v>
+      </c>
+      <c r="X919" s="12">
+        <v>1299.8</v>
+      </c>
+      <c r="Y919" s="12">
+        <v>8.4</v>
+      </c>
+      <c r="Z919" s="12">
+        <v>33.1</v>
+      </c>
+      <c r="AA919" s="13">
+        <v>307</v>
+      </c>
+      <c r="AB919" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC919" s="12">
+        <v>1005.5</v>
+      </c>
+      <c r="AD919" s="12">
+        <v>1005.2</v>
+      </c>
+      <c r="AE919" s="12">
+        <v>1006.1</v>
+      </c>
+      <c r="AF919" s="12">
+        <v>1005.5</v>
+      </c>
+      <c r="AG919" s="13">
+        <v>106396</v>
+      </c>
+      <c r="AH919" s="13">
+        <v>7560013</v>
+      </c>
+      <c r="AI919" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="920" spans="1:35" ht="18" customHeight="1">
+      <c r="A920" s="2" t="s">
+        <v>948</v>
+      </c>
+      <c r="B920" s="6">
+        <v>6.6</v>
+      </c>
+      <c r="C920" s="6">
+        <v>5.6</v>
+      </c>
+      <c r="D920" s="6">
+        <v>8</v>
+      </c>
+      <c r="E920" s="6">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="F920" s="6">
+        <v>6.4</v>
+      </c>
+      <c r="G920" s="7">
+        <v>99</v>
+      </c>
+      <c r="H920" s="7">
+        <v>99</v>
+      </c>
+      <c r="I920" s="7">
+        <v>99</v>
+      </c>
+      <c r="J920" s="6">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="K920" s="6">
+        <v>14.4</v>
+      </c>
+      <c r="L920" s="6">
+        <v>18.2</v>
+      </c>
+      <c r="M920" s="7">
+        <v>62</v>
+      </c>
+      <c r="N920" s="7">
+        <v>61</v>
+      </c>
+      <c r="O920" s="7">
+        <v>64</v>
+      </c>
+      <c r="P920" s="6">
+        <v>164.7</v>
+      </c>
+      <c r="Q920" s="7">
+        <v>1</v>
+      </c>
+      <c r="R920" s="6">
+        <v>3</v>
+      </c>
+      <c r="S920" s="6">
+        <v>14.5</v>
+      </c>
+      <c r="T920" s="6">
+        <v>272.3</v>
+      </c>
+      <c r="U920" s="6">
+        <v>0</v>
+      </c>
+      <c r="V920" s="6">
+        <v>271.3</v>
+      </c>
+      <c r="W920" s="6">
+        <v>87.1</v>
+      </c>
+      <c r="X920" s="6">
+        <v>1300.5999999999999</v>
+      </c>
+      <c r="Y920" s="6">
+        <v>8.6</v>
+      </c>
+      <c r="Z920" s="6">
+        <v>27.7</v>
+      </c>
+      <c r="AA920" s="7">
+        <v>343</v>
+      </c>
+      <c r="AB920" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC920" s="6">
+        <v>1006.2</v>
+      </c>
+      <c r="AD920" s="6">
+        <v>1005.3</v>
+      </c>
+      <c r="AE920" s="6">
+        <v>1006.8</v>
+      </c>
+      <c r="AF920" s="6">
+        <v>1006.2</v>
+      </c>
+      <c r="AG920" s="7">
+        <v>104600</v>
+      </c>
+      <c r="AH920" s="7">
+        <v>7574409</v>
+      </c>
+      <c r="AI920" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="921" spans="1:35" ht="18" customHeight="1">
+      <c r="A921" s="11" t="s">
+        <v>949</v>
+      </c>
+      <c r="B921" s="12">
+        <v>5.9</v>
+      </c>
+      <c r="C921" s="12">
+        <v>5</v>
+      </c>
+      <c r="D921" s="12">
+        <v>6.8</v>
+      </c>
+      <c r="E921" s="12">
+        <v>2.7</v>
+      </c>
+      <c r="F921" s="12">
+        <v>5.7</v>
+      </c>
+      <c r="G921" s="13">
+        <v>99</v>
+      </c>
+      <c r="H921" s="13">
+        <v>99</v>
+      </c>
+      <c r="I921" s="13">
+        <v>99</v>
+      </c>
+      <c r="J921" s="12">
+        <v>13.5</v>
+      </c>
+      <c r="K921" s="12">
+        <v>12.6</v>
+      </c>
+      <c r="L921" s="12">
+        <v>14.5</v>
+      </c>
+      <c r="M921" s="13">
+        <v>66</v>
+      </c>
+      <c r="N921" s="13">
+        <v>63</v>
+      </c>
+      <c r="O921" s="13">
+        <v>68</v>
+      </c>
+      <c r="P921" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q921" s="13">
+        <v>0</v>
+      </c>
+      <c r="R921" s="12">
+        <v>15.6</v>
+      </c>
+      <c r="S921" s="12">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="T921" s="12">
+        <v>277.89999999999998</v>
+      </c>
+      <c r="U921" s="12">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="V921" s="12">
+        <v>276.89999999999998</v>
+      </c>
+      <c r="W921" s="12">
+        <v>92.7</v>
+      </c>
+      <c r="X921" s="12">
+        <v>1306.2</v>
+      </c>
+      <c r="Y921" s="12">
+        <v>15.9</v>
+      </c>
+      <c r="Z921" s="12">
+        <v>34.9</v>
+      </c>
+      <c r="AA921" s="13">
+        <v>9</v>
+      </c>
+      <c r="AB921" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC921" s="12">
+        <v>1006.4</v>
+      </c>
+      <c r="AD921" s="12">
+        <v>1006</v>
+      </c>
+      <c r="AE921" s="12">
+        <v>1006.9</v>
+      </c>
+      <c r="AF921" s="12">
+        <v>1006.4</v>
+      </c>
+      <c r="AG921" s="13">
+        <v>104636</v>
+      </c>
+      <c r="AH921" s="13">
+        <v>7588805</v>
+      </c>
+      <c r="AI921" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="922" spans="1:35" ht="18" customHeight="1">
+      <c r="A922" s="2" t="s">
+        <v>950</v>
+      </c>
+      <c r="B922" s="6">
+        <v>5.4</v>
+      </c>
+      <c r="C922" s="6">
+        <v>4.8</v>
+      </c>
+      <c r="D922" s="6">
+        <v>5.6</v>
+      </c>
+      <c r="E922" s="6">
+        <v>2.9</v>
+      </c>
+      <c r="F922" s="6">
+        <v>5.2</v>
+      </c>
+      <c r="G922" s="7">
+        <v>99</v>
+      </c>
+      <c r="H922" s="7">
+        <v>99</v>
+      </c>
+      <c r="I922" s="7">
+        <v>99</v>
+      </c>
+      <c r="J922" s="6">
+        <v>12.3</v>
+      </c>
+      <c r="K922" s="6">
+        <v>12</v>
+      </c>
+      <c r="L922" s="6">
+        <v>12.6</v>
+      </c>
+      <c r="M922" s="7">
+        <v>69</v>
+      </c>
+      <c r="N922" s="7">
+        <v>67</v>
+      </c>
+      <c r="O922" s="7">
+        <v>70</v>
+      </c>
+      <c r="P922" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q922" s="7">
+        <v>0</v>
+      </c>
+      <c r="R922" s="6">
+        <v>15</v>
+      </c>
+      <c r="S922" s="6">
+        <v>7.8</v>
+      </c>
+      <c r="T922" s="6">
+        <v>285.7</v>
+      </c>
+      <c r="U922" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="V922" s="6">
+        <v>7.8</v>
+      </c>
+      <c r="W922" s="6">
+        <v>100.5</v>
+      </c>
+      <c r="X922" s="6">
+        <v>1314</v>
+      </c>
+      <c r="Y922" s="6">
+        <v>12.4</v>
+      </c>
+      <c r="Z922" s="6">
+        <v>34.9</v>
+      </c>
+      <c r="AA922" s="7">
+        <v>350</v>
+      </c>
+      <c r="AB922" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC922" s="6">
+        <v>1006.9</v>
+      </c>
+      <c r="AD922" s="6">
+        <v>1005.9</v>
+      </c>
+      <c r="AE922" s="6">
+        <v>1007.7</v>
+      </c>
+      <c r="AF922" s="6">
+        <v>1006.9</v>
+      </c>
+      <c r="AG922" s="7">
+        <v>106260</v>
+      </c>
+      <c r="AH922" s="7">
+        <v>7603262</v>
+      </c>
+      <c r="AI922" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="923" spans="1:35" ht="18" customHeight="1">
+      <c r="A923" s="11" t="s">
+        <v>951</v>
+      </c>
+      <c r="B923" s="12">
+        <v>5.3</v>
+      </c>
+      <c r="C923" s="12">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="D923" s="12">
+        <v>5.6</v>
+      </c>
+      <c r="E923" s="12">
+        <v>3.1</v>
+      </c>
+      <c r="F923" s="12">
+        <v>5.2</v>
+      </c>
+      <c r="G923" s="13">
+        <v>99</v>
+      </c>
+      <c r="H923" s="13">
+        <v>99</v>
+      </c>
+      <c r="I923" s="13">
+        <v>99</v>
+      </c>
+      <c r="J923" s="12">
+        <v>11.8</v>
+      </c>
+      <c r="K923" s="12">
+        <v>11.3</v>
+      </c>
+      <c r="L923" s="12">
+        <v>12.3</v>
+      </c>
+      <c r="M923" s="13">
+        <v>69</v>
+      </c>
+      <c r="N923" s="13">
+        <v>68</v>
+      </c>
+      <c r="O923" s="13">
+        <v>71</v>
+      </c>
+      <c r="P923" s="12">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="Q923" s="13">
+        <v>0</v>
+      </c>
+      <c r="R923" s="12">
+        <v>3.6</v>
+      </c>
+      <c r="S923" s="12">
+        <v>9.1</v>
+      </c>
+      <c r="T923" s="12">
+        <v>287</v>
+      </c>
+      <c r="U923" s="12">
+        <v>0</v>
+      </c>
+      <c r="V923" s="12">
+        <v>9.1</v>
+      </c>
+      <c r="W923" s="12">
+        <v>101.8</v>
+      </c>
+      <c r="X923" s="12">
+        <v>1315.3</v>
+      </c>
+      <c r="Y923" s="12">
+        <v>10.5</v>
+      </c>
+      <c r="Z923" s="12">
+        <v>25.6</v>
+      </c>
+      <c r="AA923" s="13">
+        <v>359</v>
+      </c>
+      <c r="AB923" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC923" s="12">
+        <v>1008.3</v>
+      </c>
+      <c r="AD923" s="12">
+        <v>1007.1</v>
+      </c>
+      <c r="AE923" s="12">
+        <v>1009.7</v>
+      </c>
+      <c r="AF923" s="12">
+        <v>1008.3</v>
+      </c>
+      <c r="AG923" s="13">
+        <v>106652</v>
+      </c>
+      <c r="AH923" s="13">
+        <v>7617659</v>
+      </c>
+      <c r="AI923" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="924" spans="1:35" ht="18" customHeight="1">
+      <c r="A924" s="2" t="s">
+        <v>952</v>
+      </c>
+      <c r="B924" s="6">
+        <v>6.9</v>
+      </c>
+      <c r="C924" s="6">
+        <v>5.3</v>
+      </c>
+      <c r="D924" s="6">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="E924" s="6">
+        <v>4.3</v>
+      </c>
+      <c r="F924" s="6">
+        <v>6.7</v>
+      </c>
+      <c r="G924" s="7">
+        <v>99</v>
+      </c>
+      <c r="H924" s="7">
+        <v>99</v>
+      </c>
+      <c r="I924" s="7">
+        <v>99</v>
+      </c>
+      <c r="J924" s="6">
+        <v>14.4</v>
+      </c>
+      <c r="K924" s="6">
+        <v>11.3</v>
+      </c>
+      <c r="L924" s="6">
+        <v>16.3</v>
+      </c>
+      <c r="M924" s="7">
+        <v>66</v>
+      </c>
+      <c r="N924" s="7">
+        <v>61</v>
+      </c>
+      <c r="O924" s="7">
+        <v>76</v>
+      </c>
+      <c r="P924" s="6">
+        <v>412.9</v>
+      </c>
+      <c r="Q924" s="7">
+        <v>4</v>
+      </c>
+      <c r="R924" s="6">
+        <v>0</v>
+      </c>
+      <c r="S924" s="6">
+        <v>9.1</v>
+      </c>
+      <c r="T924" s="6">
+        <v>287</v>
+      </c>
+      <c r="U924" s="6">
+        <v>0</v>
+      </c>
+      <c r="V924" s="6">
+        <v>9.1</v>
+      </c>
+      <c r="W924" s="6">
+        <v>101.8</v>
+      </c>
+      <c r="X924" s="6">
+        <v>1315.3</v>
+      </c>
+      <c r="Y924" s="6">
+        <v>14.1</v>
+      </c>
+      <c r="Z924" s="6">
+        <v>27.7</v>
+      </c>
+      <c r="AA924" s="7">
+        <v>16</v>
+      </c>
+      <c r="AB924" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC924" s="6">
+        <v>1010.8</v>
+      </c>
+      <c r="AD924" s="6">
+        <v>1009.3</v>
+      </c>
+      <c r="AE924" s="6">
+        <v>1011.9</v>
+      </c>
+      <c r="AF924" s="6">
+        <v>1010.8</v>
+      </c>
+      <c r="AG924" s="7">
+        <v>106396</v>
+      </c>
+      <c r="AH924" s="7">
+        <v>7632054</v>
+      </c>
+      <c r="AI924" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="925" spans="1:35" ht="18" customHeight="1">
+      <c r="A925" s="11" t="s">
+        <v>953</v>
+      </c>
+      <c r="B925" s="12">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="C925" s="12">
+        <v>8.4</v>
+      </c>
+      <c r="D925" s="12">
+        <v>10.8</v>
+      </c>
+      <c r="E925" s="12">
+        <v>9</v>
+      </c>
+      <c r="F925" s="12">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="G925" s="13">
+        <v>99</v>
+      </c>
+      <c r="H925" s="13">
+        <v>99</v>
+      </c>
+      <c r="I925" s="13">
+        <v>99</v>
+      </c>
+      <c r="J925" s="12">
+        <v>14.4</v>
+      </c>
+      <c r="K925" s="12">
+        <v>14</v>
+      </c>
+      <c r="L925" s="12">
+        <v>15.6</v>
+      </c>
+      <c r="M925" s="13">
+        <v>61</v>
+      </c>
+      <c r="N925" s="13">
+        <v>60</v>
+      </c>
+      <c r="O925" s="13">
+        <v>62</v>
+      </c>
+      <c r="P925" s="12">
+        <v>507.9</v>
+      </c>
+      <c r="Q925" s="13">
+        <v>4</v>
+      </c>
+      <c r="R925" s="12">
+        <v>0</v>
+      </c>
+      <c r="S925" s="12">
+        <v>9.1</v>
+      </c>
+      <c r="T925" s="12">
+        <v>287</v>
+      </c>
+      <c r="U925" s="12">
+        <v>0</v>
+      </c>
+      <c r="V925" s="12">
+        <v>9.1</v>
+      </c>
+      <c r="W925" s="12">
+        <v>101.8</v>
+      </c>
+      <c r="X925" s="12">
+        <v>1315.3</v>
+      </c>
+      <c r="Y925" s="12">
+        <v>9.1</v>
+      </c>
+      <c r="Z925" s="12">
+        <v>25.6</v>
+      </c>
+      <c r="AA925" s="13">
+        <v>357</v>
+      </c>
+      <c r="AB925" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC925" s="12">
+        <v>1011.8</v>
+      </c>
+      <c r="AD925" s="12">
+        <v>1011.3</v>
+      </c>
+      <c r="AE925" s="12">
+        <v>1012.3</v>
+      </c>
+      <c r="AF925" s="12">
+        <v>1011.8</v>
+      </c>
+      <c r="AG925" s="13">
+        <v>106640</v>
+      </c>
+      <c r="AH925" s="13">
+        <v>7646450</v>
+      </c>
+      <c r="AI925" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="926" spans="1:35" ht="18" customHeight="1">
+      <c r="A926" s="2" t="s">
+        <v>954</v>
+      </c>
+      <c r="B926" s="6">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="C926" s="6">
+        <v>6.3</v>
+      </c>
+      <c r="D926" s="6">
+        <v>10.6</v>
+      </c>
+      <c r="E926" s="6">
+        <v>7.8</v>
+      </c>
+      <c r="F926" s="6">
+        <v>8.5</v>
+      </c>
+      <c r="G926" s="7">
+        <v>99</v>
+      </c>
+      <c r="H926" s="7">
+        <v>99</v>
+      </c>
+      <c r="I926" s="7">
+        <v>99</v>
+      </c>
+      <c r="J926" s="6">
+        <v>13</v>
+      </c>
+      <c r="K926" s="6">
+        <v>11.8</v>
+      </c>
+      <c r="L926" s="6">
+        <v>14</v>
+      </c>
+      <c r="M926" s="7">
+        <v>64</v>
+      </c>
+      <c r="N926" s="7">
+        <v>61</v>
+      </c>
+      <c r="O926" s="7">
+        <v>66</v>
+      </c>
+      <c r="P926" s="6">
+        <v>163.69999999999999</v>
+      </c>
+      <c r="Q926" s="7">
+        <v>1</v>
+      </c>
+      <c r="R926" s="6">
+        <v>0</v>
+      </c>
+      <c r="S926" s="6">
+        <v>9.1</v>
+      </c>
+      <c r="T926" s="6">
+        <v>287</v>
+      </c>
+      <c r="U926" s="6">
+        <v>0</v>
+      </c>
+      <c r="V926" s="6">
+        <v>9.1</v>
+      </c>
+      <c r="W926" s="6">
+        <v>101.8</v>
+      </c>
+      <c r="X926" s="6">
+        <v>1315.3</v>
+      </c>
+      <c r="Y926" s="6">
+        <v>7.2</v>
+      </c>
+      <c r="Z926" s="6">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="AA926" s="7">
+        <v>24</v>
+      </c>
+      <c r="AB926" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC926" s="6">
+        <v>1012.9</v>
+      </c>
+      <c r="AD926" s="6">
+        <v>1011.9</v>
+      </c>
+      <c r="AE926" s="6">
+        <v>1013.6</v>
+      </c>
+      <c r="AF926" s="6">
+        <v>1012.9</v>
+      </c>
+      <c r="AG926" s="7">
+        <v>104624</v>
+      </c>
+      <c r="AH926" s="7">
+        <v>7660846</v>
+      </c>
+      <c r="AI926" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="927" spans="1:35" ht="18" customHeight="1">
+      <c r="A927" s="11" t="s">
+        <v>955</v>
+      </c>
+      <c r="B927" s="12">
+        <v>5.5</v>
+      </c>
+      <c r="C927" s="12">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="D927" s="12">
+        <v>6.6</v>
+      </c>
+      <c r="E927" s="12">
+        <v>3.5</v>
+      </c>
+      <c r="F927" s="12">
+        <v>5.3</v>
+      </c>
+      <c r="G927" s="13">
+        <v>99</v>
+      </c>
+      <c r="H927" s="13">
+        <v>99</v>
+      </c>
+      <c r="I927" s="13">
+        <v>99</v>
+      </c>
+      <c r="J927" s="12">
+        <v>11.1</v>
+      </c>
+      <c r="K927" s="12">
+        <v>10.4</v>
+      </c>
+      <c r="L927" s="12">
+        <v>11.8</v>
+      </c>
+      <c r="M927" s="13">
+        <v>66</v>
+      </c>
+      <c r="N927" s="13">
+        <v>66</v>
+      </c>
+      <c r="O927" s="13">
+        <v>67</v>
+      </c>
+      <c r="P927" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q927" s="13">
+        <v>0</v>
+      </c>
+      <c r="R927" s="12">
+        <v>0</v>
+      </c>
+      <c r="S927" s="12">
+        <v>9.1</v>
+      </c>
+      <c r="T927" s="12">
+        <v>287</v>
+      </c>
+      <c r="U927" s="12">
+        <v>0</v>
+      </c>
+      <c r="V927" s="12">
+        <v>9.1</v>
+      </c>
+      <c r="W927" s="12">
+        <v>101.8</v>
+      </c>
+      <c r="X927" s="12">
+        <v>1315.3</v>
+      </c>
+      <c r="Y927" s="12">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="Z927" s="12">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="AA927" s="13">
+        <v>59</v>
+      </c>
+      <c r="AB927" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC927" s="12">
+        <v>1013.5</v>
+      </c>
+      <c r="AD927" s="12">
+        <v>1012.8</v>
+      </c>
+      <c r="AE927" s="12">
+        <v>1014.1</v>
+      </c>
+      <c r="AF927" s="12">
+        <v>1013.5</v>
+      </c>
+      <c r="AG927" s="13">
+        <v>104600</v>
+      </c>
+      <c r="AH927" s="13">
+        <v>7675242</v>
+      </c>
+      <c r="AI927" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="928" spans="1:35" ht="18" customHeight="1">
+      <c r="A928" s="2" t="s">
+        <v>956</v>
+      </c>
+      <c r="B928" s="6">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="C928" s="6">
+        <v>4.2</v>
+      </c>
+      <c r="D928" s="6">
+        <v>5.3</v>
+      </c>
+      <c r="E928" s="6">
+        <v>3.6</v>
+      </c>
+      <c r="F928" s="6">
+        <v>4.7</v>
+      </c>
+      <c r="G928" s="7">
+        <v>99</v>
+      </c>
+      <c r="H928" s="7">
+        <v>99</v>
+      </c>
+      <c r="I928" s="7">
+        <v>99</v>
+      </c>
+      <c r="J928" s="6">
+        <v>10.3</v>
+      </c>
+      <c r="K928" s="6">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="L928" s="6">
+        <v>10.4</v>
+      </c>
+      <c r="M928" s="7">
+        <v>66</v>
+      </c>
+      <c r="N928" s="7">
+        <v>65</v>
+      </c>
+      <c r="O928" s="7">
+        <v>67</v>
+      </c>
+      <c r="P928" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q928" s="7">
+        <v>0</v>
+      </c>
+      <c r="R928" s="6">
+        <v>0</v>
+      </c>
+      <c r="S928" s="6">
+        <v>0</v>
+      </c>
+      <c r="T928" s="6">
+        <v>287</v>
+      </c>
+      <c r="U928" s="6">
+        <v>0</v>
+      </c>
+      <c r="V928" s="6">
+        <v>9.1</v>
+      </c>
+      <c r="W928" s="6">
+        <v>101.8</v>
+      </c>
+      <c r="X928" s="6">
+        <v>1315.3</v>
+      </c>
+      <c r="Y928" s="6">
+        <v>6.4</v>
+      </c>
+      <c r="Z928" s="6">
+        <v>14.8</v>
+      </c>
+      <c r="AA928" s="7">
+        <v>50</v>
+      </c>
+      <c r="AB928" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC928" s="6">
+        <v>1012.5</v>
+      </c>
+      <c r="AD928" s="6">
+        <v>1011.4</v>
+      </c>
+      <c r="AE928" s="6">
+        <v>1013.2</v>
+      </c>
+      <c r="AF928" s="6">
+        <v>1012.5</v>
+      </c>
+      <c r="AG928" s="7">
+        <v>106608</v>
+      </c>
+      <c r="AH928" s="7">
+        <v>7689638</v>
+      </c>
+      <c r="AI928" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="929" spans="1:35" ht="18" customHeight="1">
+      <c r="A929" s="16" t="s">
+        <v>957</v>
+      </c>
+      <c r="B929" s="17">
+        <v>5.8</v>
+      </c>
+      <c r="C929" s="17">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="D929" s="17">
+        <v>7.4</v>
+      </c>
+      <c r="E929" s="17">
+        <v>5.6</v>
+      </c>
+      <c r="F929" s="17">
+        <v>5.7</v>
+      </c>
+      <c r="G929" s="18">
+        <v>99</v>
+      </c>
+      <c r="H929" s="18">
+        <v>99</v>
+      </c>
+      <c r="I929" s="18">
+        <v>99</v>
+      </c>
+      <c r="J929" s="17">
+        <v>10.4</v>
+      </c>
+      <c r="K929" s="17">
+        <v>10.1</v>
+      </c>
+      <c r="L929" s="17">
+        <v>10.7</v>
+      </c>
+      <c r="M929" s="18">
+        <v>66</v>
+      </c>
+      <c r="N929" s="18">
+        <v>65</v>
+      </c>
+      <c r="O929" s="18">
+        <v>67</v>
+      </c>
+      <c r="P929" s="17">
+        <v>1.2</v>
+      </c>
+      <c r="Q929" s="18">
+        <v>0</v>
+      </c>
+      <c r="R929" s="17">
+        <v>0</v>
+      </c>
+      <c r="S929" s="17">
+        <v>0</v>
+      </c>
+      <c r="T929" s="17">
+        <v>287</v>
+      </c>
+      <c r="U929" s="17">
+        <v>0</v>
+      </c>
+      <c r="V929" s="17">
+        <v>9.1</v>
+      </c>
+      <c r="W929" s="17">
+        <v>101.8</v>
+      </c>
+      <c r="X929" s="17">
+        <v>1315.3</v>
+      </c>
+      <c r="Y929" s="17">
+        <v>3.1</v>
+      </c>
+      <c r="Z929" s="17">
+        <v>7.2</v>
+      </c>
+      <c r="AA929" s="18">
+        <v>42</v>
+      </c>
+      <c r="AB929" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC929" s="17">
+        <v>1011</v>
+      </c>
+      <c r="AD929" s="17">
+        <v>1010.1</v>
+      </c>
+      <c r="AE929" s="17">
+        <v>1011.8</v>
+      </c>
+      <c r="AF929" s="17">
+        <v>1011</v>
+      </c>
+      <c r="AG929" s="18">
+        <v>106632</v>
+      </c>
+      <c r="AH929" s="18">
+        <v>7704034</v>
+      </c>
+      <c r="AI929" s="20">
         <v>0</v>
       </c>
     </row>

</xml_diff>